<commit_message>
Lectures; macro1 hw; typos
</commit_message>
<xml_diff>
--- a/1/finance_1/Excel Class Exercise Lecture 1.xlsx
+++ b/1/finance_1/Excel Class Exercise Lecture 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgenkin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mellanox365-my.sharepoint.com/personal/lgenkin_mellanox_com/Documents/Documents/mafe/1/finance_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF063A5F-8CC8-4C35-B2F3-888925428700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{EF063A5F-8CC8-4C35-B2F3-888925428700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8868F61-0405-4EE8-9D92-6D5F074ADD30}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="824" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Class Exercise 1 - Page 14" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -679,58 +679,61 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1314,29 +1317,29 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1383,123 +1386,155 @@
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:17" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="51"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="56"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="19"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B9" s="19">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <f>PV(B9, B10, B11)</f>
+        <v>-1067477.6188588582</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="19"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="19">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <f>B12</f>
+        <v>-1067477.6188588582</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <f>PV(B16, B17, 0, B18)</f>
+        <v>494448.68173156766</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="19"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="19">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <f>B19</f>
+        <v>494448.68173156766</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4">
+        <f>PMT(B23, B24, 0, B25)</f>
+        <v>-6763.4542699430276</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1515,54 +1550,68 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:10" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="46"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="19"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="19">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="32">
+        <f>B5*(1+B3/B6)^(B6*B4)</f>
+        <v>662.04089516146541</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1575,99 +1624,131 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85104D98-E4FC-443B-BB75-16E85D981041}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="73.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:12" ht="73.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="46"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="51"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="19"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="19">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <f>(1+B10/B11)^(B11/B12)-1</f>
+        <v>3.0300999999999911E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <f>B14</f>
+        <v>3.0300999999999911E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <f>30*4</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="33">
+        <f>PMT(B17,B18,B19)</f>
+        <v>-3116.799029943963</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="33">
+        <f>B20*120</f>
+        <v>-374015.88359327556</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1686,45 +1767,45 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="9"/>
-    <col min="2" max="2" width="9.6328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.08984375" style="9"/>
+    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="2" max="2" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:12" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="41"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="46"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -1732,7 +1813,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
@@ -1740,7 +1821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -1748,7 +1829,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
@@ -1757,12 +1838,12 @@
         <v>220.50895583893598</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
@@ -1770,7 +1851,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
@@ -1778,7 +1859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
@@ -1786,7 +1867,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>3</v>
       </c>
@@ -1812,37 +1893,37 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="6" customWidth="1"/>
-    <col min="2" max="2" width="16.08984375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="24.08984375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="9.08984375" style="6"/>
+    <col min="2" max="2" width="16.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="42" t="s">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="47" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>0</v>
       </c>
@@ -1857,7 +1938,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>1</v>
       </c>
@@ -1872,7 +1953,7 @@
         <v>185.18518518518516</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>2</v>
       </c>
@@ -1887,7 +1968,7 @@
         <v>1286.0082304526748</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>3</v>
       </c>
@@ -1902,20 +1983,20 @@
         <v>1587.6644820403392</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D11" s="52">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="36">
         <f>SUM(D7:D10)</f>
         <v>2058.8578976781992</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="17">
         <v>0.08</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="37">
         <f>NPV(B12, B8:B10)+B7</f>
         <v>2058.8578976781992</v>
       </c>
@@ -1936,38 +2017,38 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:12" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="51"/>
       <c r="L1" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -1993,7 +2074,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>-1000</v>
@@ -2011,17 +2092,17 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2029,7 +2110,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2037,7 +2118,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2045,10 +2126,10 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2057,7 +2138,7 @@
         <v>259056.51870999858</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2077,35 +2158,35 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="49"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="54"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2131,7 +2212,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="20" t="s">
         <v>27</v>
@@ -2149,17 +2230,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2167,7 +2248,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2175,7 +2256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2183,7 +2264,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2192,7 +2273,7 @@
         <v>2901.6322803399003</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2216,33 +2297,33 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:9" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="46"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -2268,7 +2349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="20">
         <v>5000</v>
@@ -2286,26 +2367,26 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="22"/>
-      <c r="C11" s="54">
+      <c r="C11" s="38">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2313,7 +2394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2321,7 +2402,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2330,7 +2411,7 @@
         <v>55734.729303311236</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2352,43 +2433,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" customWidth="1"/>
-    <col min="7" max="7" width="18.08984375" customWidth="1"/>
-    <col min="8" max="11" width="15.36328125" customWidth="1"/>
-    <col min="12" max="12" width="19.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:12" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="46"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="51"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>36</v>
       </c>
@@ -2413,7 +2494,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>0</v>
       </c>
@@ -2438,12 +2519,12 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2451,7 +2532,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2459,7 +2540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2467,17 +2548,17 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="55">
+      <c r="B15" s="39">
         <f>B13/((1-(1/(1+B11)^B12))/B11)</f>
         <v>7913.9244238423562</v>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2487,12 +2568,12 @@
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20" s="26" t="s">
         <v>13</v>
       </c>
@@ -2512,7 +2593,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>1</v>
       </c>
@@ -2523,7 +2604,7 @@
         <f>7913.92</f>
         <v>7913.92</v>
       </c>
-      <c r="I21" s="55">
+      <c r="I21" s="39">
         <f>G21*B11</f>
         <v>3000</v>
       </c>
@@ -2536,7 +2617,7 @@
         <v>25086.080000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>2</v>
       </c>
@@ -2561,7 +2642,7 @@
         <v>19680.768000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>3</v>
       </c>
@@ -2586,7 +2667,7 @@
         <v>13734.924800000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>4</v>
       </c>
@@ -2611,7 +2692,7 @@
         <v>7194.497280000005</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>5</v>
       </c>
@@ -2651,37 +2732,37 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:11" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="51"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2689,7 +2770,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2697,7 +2778,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2705,17 +2786,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="39">
         <f>B7/B6</f>
         <v>1000</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2735,37 +2816,37 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5BD424-01C8-4084-B091-4754AEB2C3BD}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" style="31" customWidth="1"/>
-    <col min="3" max="4" width="20.81640625" style="31" customWidth="1"/>
-    <col min="5" max="7" width="8.36328125" style="31" customWidth="1"/>
-    <col min="8" max="16384" width="12.1796875" style="31"/>
+    <col min="1" max="1" width="20.85546875" style="31" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="31" customWidth="1"/>
+    <col min="3" max="4" width="20.85546875" style="31" customWidth="1"/>
+    <col min="5" max="7" width="8.42578125" style="31" customWidth="1"/>
+    <col min="8" max="16384" width="12.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:7" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="56"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="31">
         <v>1</v>
       </c>
@@ -2782,7 +2863,7 @@
         <v>1.1576250000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="31">
         <v>0</v>
       </c>
@@ -2802,12 +2883,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>1</v>
       </c>
@@ -2815,7 +2896,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>69</v>
       </c>
@@ -2823,7 +2904,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>29</v>
       </c>
@@ -2831,13 +2912,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="35">
         <f>B11/(B9-B10)</f>
         <v>33.333333333333336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="40">
+        <f>FV(1%,10,100)</f>
+        <v>-1046.2212541120473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>